<commit_message>
GoodInfo_v2 - 2021.12.07 未完成
</commit_message>
<xml_diff>
--- a/持股分析_2021-12-07_LOST.xlsx
+++ b/持股分析_2021-12-07_LOST.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN7"/>
+  <dimension ref="A1:AO7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,135 +496,140 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>代號</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Class_x</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>一年最高股價_x</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>3日分數_x</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>5日分數_x</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>連續分數_x</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Type_x</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>距離最高點_x</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">	類別_y</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">	庫存股數_y</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">	持有成本_y</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">	成交均價_y</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">	現價_y</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">	股票現值_y</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">	未實現損益_y</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">	預估報酬率_y</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">	手續費_y</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">	交易稅_y</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">	幣別_y</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Class_y</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>一年最高股價_y</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>3日分數_y</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>5日分數_y</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>連續分數_y</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Type_y</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>距離最高點_y</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>_merge</t>
         </is>
@@ -681,64 +686,65 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr">
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr">
         <is>
           <t>LOST</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="n">
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="n">
         <v>20</v>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>現股</t>
         </is>
       </c>
-      <c r="W2" t="n">
+      <c r="X2" t="n">
         <v>7</v>
       </c>
-      <c r="X2" t="n">
+      <c r="Y2" t="n">
         <v>1586</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="Z2" t="n">
         <v>226.5</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="AA2" t="n">
         <v>213</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AB2" t="n">
         <v>1486</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AC2" t="n">
         <v>-100</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AD2" t="n">
         <v>-0.0631</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AE2" t="n">
         <v>1</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AF2" t="n">
         <v>4</v>
       </c>
-      <c r="AF2" t="inlineStr">
+      <c r="AG2" t="inlineStr">
         <is>
           <t>台幣</t>
         </is>
       </c>
-      <c r="AG2" t="inlineStr"/>
       <c r="AH2" t="inlineStr"/>
       <c r="AI2" t="inlineStr"/>
       <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="inlineStr">
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr">
         <is>
           <t>LOST</t>
         </is>
       </c>
-      <c r="AM2" t="inlineStr"/>
-      <c r="AN2" t="inlineStr">
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr">
         <is>
           <t>both</t>
         </is>
@@ -795,64 +801,65 @@
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr">
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr">
         <is>
           <t>LOST</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="n">
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="n">
         <v>0</v>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="W3" t="inlineStr">
         <is>
           <t>現股</t>
         </is>
       </c>
-      <c r="W3" t="n">
+      <c r="X3" t="n">
         <v>54</v>
       </c>
-      <c r="X3" t="n">
+      <c r="Y3" t="n">
         <v>1499</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="Z3" t="n">
         <v>27.75</v>
       </c>
-      <c r="Z3" t="n">
+      <c r="AA3" t="n">
         <v>27.7</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AB3" t="n">
         <v>1490</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="AC3" t="n">
         <v>-9</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="AD3" t="n">
         <v>-0.006</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="AE3" t="n">
         <v>1</v>
       </c>
-      <c r="AE3" t="n">
+      <c r="AF3" t="n">
         <v>4</v>
       </c>
-      <c r="AF3" t="inlineStr">
+      <c r="AG3" t="inlineStr">
         <is>
           <t>台幣</t>
         </is>
       </c>
-      <c r="AG3" t="inlineStr"/>
       <c r="AH3" t="inlineStr"/>
       <c r="AI3" t="inlineStr"/>
       <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="inlineStr">
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr">
         <is>
           <t>LOST</t>
         </is>
       </c>
-      <c r="AM3" t="inlineStr"/>
-      <c r="AN3" t="inlineStr">
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr">
         <is>
           <t>both</t>
         </is>
@@ -909,64 +916,65 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr">
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr">
         <is>
           <t>LOST</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="n">
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="n">
         <v>15</v>
       </c>
-      <c r="V4" t="inlineStr">
+      <c r="W4" t="inlineStr">
         <is>
           <t>現股</t>
         </is>
       </c>
-      <c r="W4" t="n">
+      <c r="X4" t="n">
         <v>37</v>
       </c>
-      <c r="X4" t="n">
+      <c r="Y4" t="n">
         <v>1481</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="Z4" t="n">
         <v>40</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="AA4" t="n">
         <v>40.6</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AB4" t="n">
         <v>1497</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="AC4" t="n">
         <v>16</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="AD4" t="n">
         <v>0.0108</v>
       </c>
-      <c r="AD4" t="n">
+      <c r="AE4" t="n">
         <v>1</v>
       </c>
-      <c r="AE4" t="n">
+      <c r="AF4" t="n">
         <v>4</v>
       </c>
-      <c r="AF4" t="inlineStr">
+      <c r="AG4" t="inlineStr">
         <is>
           <t>台幣</t>
         </is>
       </c>
-      <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="inlineStr"/>
       <c r="AI4" t="inlineStr"/>
       <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="inlineStr"/>
-      <c r="AL4" t="inlineStr">
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr">
         <is>
           <t>LOST</t>
         </is>
       </c>
-      <c r="AM4" t="inlineStr"/>
-      <c r="AN4" t="inlineStr">
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr">
         <is>
           <t>both</t>
         </is>
@@ -1023,64 +1031,65 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr">
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr">
         <is>
           <t>LOST</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" t="n">
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="n">
         <v>12</v>
       </c>
-      <c r="V5" t="inlineStr">
+      <c r="W5" t="inlineStr">
         <is>
           <t>現股</t>
         </is>
       </c>
-      <c r="W5" t="n">
+      <c r="X5" t="n">
         <v>7</v>
       </c>
-      <c r="X5" t="n">
+      <c r="Y5" t="n">
         <v>2987</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="Z5" t="n">
         <v>426.43</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="AA5" t="n">
         <v>430</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AB5" t="n">
         <v>3000</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AC5" t="n">
         <v>13</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="AD5" t="n">
         <v>0.0044</v>
       </c>
-      <c r="AD5" t="n">
+      <c r="AE5" t="n">
         <v>2</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AF5" t="n">
         <v>8</v>
       </c>
-      <c r="AF5" t="inlineStr">
+      <c r="AG5" t="inlineStr">
         <is>
           <t>台幣</t>
         </is>
       </c>
-      <c r="AG5" t="inlineStr"/>
       <c r="AH5" t="inlineStr"/>
       <c r="AI5" t="inlineStr"/>
       <c r="AJ5" t="inlineStr"/>
       <c r="AK5" t="inlineStr"/>
-      <c r="AL5" t="inlineStr">
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr">
         <is>
           <t>LOST</t>
         </is>
       </c>
-      <c r="AM5" t="inlineStr"/>
-      <c r="AN5" t="inlineStr">
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr">
         <is>
           <t>both</t>
         </is>
@@ -1137,64 +1146,65 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr">
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr">
         <is>
           <t>LOST</t>
         </is>
       </c>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="n">
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="n">
         <v>10</v>
       </c>
-      <c r="V6" t="inlineStr">
+      <c r="W6" t="inlineStr">
         <is>
           <t>現股</t>
         </is>
       </c>
-      <c r="W6" t="n">
+      <c r="X6" t="n">
         <v>6</v>
       </c>
-      <c r="X6" t="n">
+      <c r="Y6" t="n">
         <v>1489</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="Z6" t="n">
         <v>248</v>
       </c>
-      <c r="Z6" t="n">
+      <c r="AA6" t="n">
         <v>246</v>
       </c>
-      <c r="AA6" t="n">
+      <c r="AB6" t="n">
         <v>1471</v>
       </c>
-      <c r="AB6" t="n">
+      <c r="AC6" t="n">
         <v>-18</v>
       </c>
-      <c r="AC6" t="n">
+      <c r="AD6" t="n">
         <v>-0.0121</v>
       </c>
-      <c r="AD6" t="n">
+      <c r="AE6" t="n">
         <v>1</v>
       </c>
-      <c r="AE6" t="n">
+      <c r="AF6" t="n">
         <v>4</v>
       </c>
-      <c r="AF6" t="inlineStr">
+      <c r="AG6" t="inlineStr">
         <is>
           <t>台幣</t>
         </is>
       </c>
-      <c r="AG6" t="inlineStr"/>
       <c r="AH6" t="inlineStr"/>
       <c r="AI6" t="inlineStr"/>
       <c r="AJ6" t="inlineStr"/>
       <c r="AK6" t="inlineStr"/>
-      <c r="AL6" t="inlineStr">
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr">
         <is>
           <t>LOST</t>
         </is>
       </c>
-      <c r="AM6" t="inlineStr"/>
-      <c r="AN6" t="inlineStr">
+      <c r="AN6" t="inlineStr"/>
+      <c r="AO6" t="inlineStr">
         <is>
           <t>both</t>
         </is>
@@ -1251,64 +1261,65 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr">
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr">
         <is>
           <t>LOST</t>
         </is>
       </c>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="n">
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="n">
         <v>9</v>
       </c>
-      <c r="V7" t="inlineStr">
+      <c r="W7" t="inlineStr">
         <is>
           <t>現股</t>
         </is>
       </c>
-      <c r="W7" t="n">
+      <c r="X7" t="n">
         <v>22</v>
       </c>
-      <c r="X7" t="n">
+      <c r="Y7" t="n">
         <v>1508</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="Z7" t="n">
         <v>68.5</v>
       </c>
-      <c r="Z7" t="n">
+      <c r="AA7" t="n">
         <v>71.09999999999999</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AB7" t="n">
         <v>1559</v>
       </c>
-      <c r="AB7" t="n">
+      <c r="AC7" t="n">
         <v>51</v>
       </c>
-      <c r="AC7" t="n">
+      <c r="AD7" t="n">
         <v>0.0338</v>
       </c>
-      <c r="AD7" t="n">
+      <c r="AE7" t="n">
         <v>1</v>
       </c>
-      <c r="AE7" t="n">
+      <c r="AF7" t="n">
         <v>4</v>
       </c>
-      <c r="AF7" t="inlineStr">
+      <c r="AG7" t="inlineStr">
         <is>
           <t>台幣</t>
         </is>
       </c>
-      <c r="AG7" t="inlineStr"/>
       <c r="AH7" t="inlineStr"/>
       <c r="AI7" t="inlineStr"/>
       <c r="AJ7" t="inlineStr"/>
       <c r="AK7" t="inlineStr"/>
-      <c r="AL7" t="inlineStr">
+      <c r="AL7" t="inlineStr"/>
+      <c r="AM7" t="inlineStr">
         <is>
           <t>LOST</t>
         </is>
       </c>
-      <c r="AM7" t="inlineStr"/>
-      <c r="AN7" t="inlineStr">
+      <c r="AN7" t="inlineStr"/>
+      <c r="AO7" t="inlineStr">
         <is>
           <t>both</t>
         </is>

</xml_diff>